<commit_message>
Scaling updates to better match EMEP, etc.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -311,7 +311,13 @@
     <t>all</t>
   </si>
   <si>
-    <t>Don't scale to 1990-1991 drop so as to be closer to EMEP trend</t>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>Don't scale 1981 to avoid reporting mistake in inventory</t>
+  </si>
+  <si>
+    <t>Scale from 2000 so as to be closer to EMEP trend</t>
   </si>
 </sst>
 </file>
@@ -367,8 +373,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -613,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -732,6 +758,16 @@
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -850,6 +886,16 @@
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1186,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2139,15 +2185,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2170,10 +2216,13 @@
         <v>92</v>
       </c>
       <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -2190,13 +2239,45 @@
         <v>7</v>
       </c>
       <c r="F2">
-        <v>1990</v>
+        <v>2000</v>
       </c>
       <c r="G2">
         <v>2010</v>
       </c>
       <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>1982</v>
+      </c>
+      <c r="G3">
+        <v>2020</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix scaling error when expanding 'all'. Now picks most specific instruction and keeps last row.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
+++ b/input/mappings/scaling/EMEP_NFR09_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="2280" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="100">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -2130,7 +2130,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2190,7 +2189,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2201,15 +2199,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2232,13 +2230,10 @@
         <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -2261,13 +2256,10 @@
         <v>2010</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -2290,13 +2282,10 @@
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2319,15 +2308,11 @@
         <v>2020</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>